<commit_message>
ADD: Change credential managment and storage.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\NeostellaAutomationTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2211F45F-F63D-4C37-AD4B-CFF7EE9AE683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CEC6D4-42B5-4C2D-BC3B-F8BE9D04E134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -162,18 +162,6 @@
     <t>=============== Initialization Constants ===============</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>jmonsalveb@unal.edu.co</t>
-  </si>
-  <si>
-    <t>BxRTZTTZpLp4!qJ</t>
-  </si>
-  <si>
     <t>https://acme-test.uipath.com/</t>
   </si>
   <si>
@@ -244,6 +232,12 @@
   </si>
   <si>
     <t>Data\Downloads\</t>
+  </si>
+  <si>
+    <t>ACME_CredentialAssetNameInWindowsCredentialsManager</t>
+  </si>
+  <si>
+    <t>ACMESystem1_Credential</t>
   </si>
 </sst>
 </file>
@@ -637,15 +631,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="55.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
@@ -769,7 +763,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>22</v>
@@ -790,124 +784,117 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
+        <v>69</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
     </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>65</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>63</v>
+      <c r="A24" t="s">
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A25" t="s">
-        <v>65</v>
+      <c r="A25" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C25" s="6"/>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="6"/>
-    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1887,12 +1874,11 @@
     <row r="1003" ht="14.25" customHeight="1"/>
     <row r="1004" ht="14.25" customHeight="1"/>
     <row r="1005" ht="14.25" customHeight="1"/>
-    <row r="1006" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:C3"/>
     <mergeCell ref="A9:C10"/>
-    <mergeCell ref="A18:C19"/>
+    <mergeCell ref="A17:C18"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATE: Remove Excel file generated with the document extraction.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\NeostellaAutomationTest\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CEC6D4-42B5-4C2D-BC3B-F8BE9D04E134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0F9C9A-4706-41F1-94D2-42C15C6BC51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1890,7 +1890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>